<commit_message>
weights and joint model
</commit_message>
<xml_diff>
--- a/Gantt project planner1.xlsx
+++ b/Gantt project planner1.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF58AA56-538A-44B9-A226-F76C8F81A795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D753099-1FAB-4770-82F3-5A03E8623CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>ACTIVITY</t>
   </si>
   <si>
-    <t>Activity 13</t>
-  </si>
-  <si>
     <t>Activity 14</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t>Revisión de nuevos proyectos</t>
+  </si>
+  <si>
+    <t>Unión de Redes</t>
   </si>
 </sst>
 </file>
@@ -1050,8 +1050,8 @@
   </sheetPr>
   <dimension ref="B1:BO32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AJ18" sqref="AJ18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B3" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1077,21 +1077,21 @@
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
       <c r="G2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" s="14">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J2" s="15"/>
       <c r="K2" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L2" s="31"/>
       <c r="M2" s="31"/>
@@ -1099,21 +1099,21 @@
       <c r="O2" s="32"/>
       <c r="P2" s="16"/>
       <c r="Q2" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R2" s="33"/>
       <c r="S2" s="33"/>
       <c r="T2" s="32"/>
       <c r="U2" s="17"/>
       <c r="V2" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W2" s="24"/>
       <c r="X2" s="24"/>
       <c r="Y2" s="34"/>
       <c r="Z2" s="18"/>
       <c r="AA2" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AB2" s="24"/>
       <c r="AC2" s="24"/>
@@ -1123,7 +1123,7 @@
       <c r="AG2" s="34"/>
       <c r="AH2" s="19"/>
       <c r="AI2" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AJ2" s="24"/>
       <c r="AK2" s="24"/>
@@ -1138,19 +1138,19 @@
         <v>2</v>
       </c>
       <c r="C3" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="F3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="G3" s="29" t="s">
         <v>24</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>25</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>1</v>
@@ -1365,7 +1365,7 @@
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="7">
         <v>2</v>
@@ -1405,7 +1405,7 @@
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="7">
         <v>2</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="7">
         <v>4</v>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="7">
         <v>4</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="7">
         <v>4</v>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="7">
         <v>7</v>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="7">
         <v>8</v>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="7">
         <v>11</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="7">
         <v>18</v>
@@ -1574,18 +1574,18 @@
         <v>6</v>
       </c>
       <c r="E15" s="7">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F15" s="7">
         <v>6</v>
       </c>
       <c r="G15" s="8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="7">
         <v>18</v>
@@ -1594,7 +1594,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="7">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F16" s="7">
         <v>4</v>
@@ -1605,7 +1605,7 @@
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="7">
         <v>22</v>
@@ -1614,7 +1614,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="7">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" s="7">
         <v>2</v>
@@ -1625,27 +1625,27 @@
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="22" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="C18" s="7">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D18" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" s="7">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F18" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18" s="8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19" s="7">
         <v>0</v>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="7">
         <v>0</v>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" s="7">
         <v>0</v>
@@ -1705,7 +1705,7 @@
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="7">
         <v>0</v>
@@ -1725,7 +1725,7 @@
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" s="7">
         <v>0</v>
@@ -1745,7 +1745,7 @@
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24" s="7">
         <v>0</v>
@@ -1765,7 +1765,7 @@
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25" s="7">
         <v>0</v>
@@ -1785,7 +1785,7 @@
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26" s="7">
         <v>0</v>
@@ -1805,7 +1805,7 @@
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C27" s="7">
         <v>0</v>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C28" s="7">
         <v>0</v>
@@ -1845,7 +1845,7 @@
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29" s="7">
         <v>0</v>
@@ -1865,7 +1865,7 @@
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" s="7">
         <v>0</v>
@@ -1885,7 +1885,7 @@
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31" s="7">
         <v>0</v>

</xml_diff>